<commit_message>
added ui and few changes for this
</commit_message>
<xml_diff>
--- a/billing/in/last_rate_file.xlsx
+++ b/billing/in/last_rate_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t xml:space="preserve">Product</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Valencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">baba</t>
   </si>
 </sst>
 </file>
@@ -70,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,48 +155,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>112</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -200,10 +201,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>104</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -211,10 +212,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>84</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -222,10 +223,10 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>92</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -233,10 +234,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>113</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -244,10 +245,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>88</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -255,10 +256,10 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -272,7 +273,7 @@
       <c r="B10" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>43</v>
       </c>
     </row>
@@ -283,7 +284,7 @@
       <c r="B11" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>45</v>
       </c>
     </row>
@@ -294,7 +295,7 @@
       <c r="B12" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>12</v>
       </c>
     </row>
@@ -305,7 +306,18 @@
       <c r="B13" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="C14" s="0" t="n">
         <v>45</v>
       </c>
     </row>

</xml_diff>